<commit_message>
Modified Generic Class functions and included Runmodes.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Datafile.xlsx
+++ b/src/test/resources/excel/Datafile.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clintonr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE749700-4A9D-43B7-9802-241792DD202C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBA90F3-3510-4DD0-8826-890C41800129}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{73745407-E88A-4B66-92CF-1C7ED9DB62D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{73745407-E88A-4B66-92CF-1C7ED9DB62D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
-    <sheet name="ListConfig" sheetId="3" r:id="rId3"/>
+    <sheet name="TestCases" sheetId="4" r:id="rId3"/>
+    <sheet name="ListConfig" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Field_Name</t>
   </si>
@@ -117,6 +118,27 @@
   </si>
   <si>
     <t>Input_Data3</t>
+  </si>
+  <si>
+    <t>TestNames</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>LoginAsBankManager</t>
+  </si>
+  <si>
+    <t>AddCustomers</t>
+  </si>
+  <si>
+    <t>OpenAccount</t>
   </si>
 </sst>
 </file>
@@ -184,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -197,6 +219,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,9 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACE8467-F6EE-4BDE-A81C-CB91895AAB67}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -590,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B432CE38-5599-4608-9732-9335A68D1F40}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -690,11 +716,73 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA41A9-03EA-4707-BD77-F3FB0B5473FD}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7D8CD784-B46B-4447-B1DC-B654482947F8}">
+          <x14:formula1>
+            <xm:f>ListConfig!$D$1:$D$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA67EEB-3B95-4B4F-A9A4-6D8671B1C555}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +792,7 @@
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -714,8 +802,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -725,8 +816,11 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Updated Framework to run cases individually.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Datafile.xlsx
+++ b/src/test/resources/excel/Datafile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clintonr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBA90F3-3510-4DD0-8826-890C41800129}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841A5DCB-FF3E-463B-9F76-34033A4B766E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{73745407-E88A-4B66-92CF-1C7ED9DB62D3}"/>
   </bookViews>
@@ -542,7 +542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACE8467-F6EE-4BDE-A81C-CB91895AAB67}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -756,7 +758,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>